<commit_message>
new people in teams
</commit_message>
<xml_diff>
--- a/data/teams.xlsx
+++ b/data/teams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivana_Kovacova\Documents\fitness challenge\fitness_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A77AD8-542C-44CC-8F9E-8B6D0AC19FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB73F7F-B4AE-41A5-B8E5-512A46E124B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{36C607E6-452E-4748-A98C-75BADCF1880B}"/>
+    <workbookView xWindow="-3732" yWindow="-17388" windowWidth="30936" windowHeight="16896" xr2:uid="{36C607E6-452E-4748-A98C-75BADCF1880B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>Fernanda Nicolao Mattei</t>
   </si>
@@ -334,6 +334,12 @@
   </si>
   <si>
     <t>J's Kaarmaa</t>
+  </si>
+  <si>
+    <t>Souvik Nath</t>
+  </si>
+  <si>
+    <t>Akhilesh Paliwal</t>
   </si>
 </sst>
 </file>
@@ -708,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885D685E-B0E0-4CBC-A964-0E9181FE0B92}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1034,6 +1040,14 @@
       </c>
       <c r="J10" s="2" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>